<commit_message>
Initial commit for Ripon model
</commit_message>
<xml_diff>
--- a/Betting_Simulation/grouped_r_metrics.xlsx
+++ b/Betting_Simulation/grouped_r_metrics.xlsx
@@ -474,20 +474,18 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-3</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -496,19 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C3" t="n">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="D3" t="n">
-        <v>136</v>
+        <v>43</v>
       </c>
       <c r="E3" t="n">
-        <v>-80</v>
+        <v>-26</v>
       </c>
       <c r="F3" t="n">
-        <v>20</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="4">
@@ -518,18 +516,20 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
+        <v>-6</v>
+      </c>
+      <c r="F4" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -649,20 +649,18 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-5</v>
-      </c>
-      <c r="F2" t="n">
-        <v>16.7</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -671,20 +669,18 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>-17</v>
-      </c>
-      <c r="F3" t="n">
-        <v>10.5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -693,20 +689,18 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>-29</v>
-      </c>
-      <c r="F4" t="n">
-        <v>19.4</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -715,19 +709,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" t="n">
-        <v>37.5</v>
+        <v>33</v>
       </c>
       <c r="D5" t="n">
-        <v>69.5</v>
+        <v>65</v>
       </c>
       <c r="E5" t="n">
         <v>-32</v>
       </c>
       <c r="F5" t="n">
-        <v>23.8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
@@ -884,23 +878,23 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>NEWMARKET</t>
+          <t>NEWBURY</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>103</v>
+        <v>40</v>
       </c>
       <c r="C2" t="n">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="D2" t="n">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="E2" t="n">
-        <v>-83</v>
+        <v>-32</v>
       </c>
       <c r="F2" t="n">
-        <v>19.4</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>